<commit_message>
update features from Yim
</commit_message>
<xml_diff>
--- a/Model_features.xlsx
+++ b/Model_features.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25330"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hle\Documents\GitHub\exe-epi-mmb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Desktop\Macroepi\Mile2\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0AB9EABA-01FA-4C57-AEBF-04CCC6DC6E2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="375" yWindow="390" windowWidth="10650" windowHeight="10755"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -19,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="85">
   <si>
     <t>exogenous SIR</t>
   </si>
@@ -284,17 +277,20 @@
   </si>
   <si>
     <t>LFA_22</t>
+  </si>
+  <si>
+    <t>Quarterly</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -302,7 +298,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Tahoma"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -616,7 +612,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -624,39 +620,39 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
       <pane xSplit="1" topLeftCell="M1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="A25" sqref="A25"/>
+      <selection pane="topRight" activeCell="M17" sqref="M17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.25" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="35.7109375" customWidth="1"/>
-    <col min="3" max="3" width="26.7109375" customWidth="1"/>
-    <col min="4" max="4" width="28.7109375" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="1" max="2" width="35.75" customWidth="1"/>
+    <col min="3" max="3" width="26.75" customWidth="1"/>
+    <col min="4" max="4" width="28.75" customWidth="1"/>
+    <col min="5" max="5" width="22.375" customWidth="1"/>
     <col min="6" max="6" width="28" customWidth="1"/>
-    <col min="7" max="7" width="19.7109375" customWidth="1"/>
-    <col min="8" max="8" width="36.7109375" customWidth="1"/>
-    <col min="9" max="9" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="19.75" customWidth="1"/>
+    <col min="8" max="8" width="36.75" customWidth="1"/>
+    <col min="9" max="9" width="30.375" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="35" customWidth="1"/>
-    <col min="11" max="11" width="43.85546875" customWidth="1"/>
-    <col min="12" max="12" width="44.7109375" customWidth="1"/>
+    <col min="11" max="11" width="43.875" customWidth="1"/>
+    <col min="12" max="12" width="44.75" customWidth="1"/>
     <col min="13" max="13" width="25" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="23.140625" customWidth="1"/>
-    <col min="15" max="15" width="22.7109375" customWidth="1"/>
-    <col min="16" max="16" width="24.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17.28515625" customWidth="1"/>
-    <col min="19" max="19" width="19.7109375" customWidth="1"/>
-    <col min="20" max="20" width="16.7109375" customWidth="1"/>
-    <col min="21" max="21" width="16.42578125" customWidth="1"/>
+    <col min="14" max="14" width="23.125" customWidth="1"/>
+    <col min="15" max="15" width="22.75" customWidth="1"/>
+    <col min="16" max="16" width="24.25" customWidth="1"/>
+    <col min="17" max="17" width="15.75" customWidth="1"/>
+    <col min="18" max="18" width="17.25" customWidth="1"/>
+    <col min="19" max="19" width="19.75" customWidth="1"/>
+    <col min="20" max="20" width="16.75" customWidth="1"/>
+    <col min="21" max="21" width="16.375" customWidth="1"/>
     <col min="22" max="22" width="19" customWidth="1"/>
-    <col min="23" max="23" width="17.42578125" customWidth="1"/>
-    <col min="24" max="24" width="21.28515625" customWidth="1"/>
+    <col min="23" max="23" width="17.375" customWidth="1"/>
+    <col min="24" max="24" width="21.25" customWidth="1"/>
     <col min="25" max="25" width="19" customWidth="1"/>
-    <col min="26" max="26" width="13.7109375" customWidth="1"/>
+    <col min="26" max="26" width="13.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -674,7 +670,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>62</v>
       </c>
@@ -691,13 +687,13 @@
         <v>58</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>59</v>
       </c>
       <c r="X3" s="1"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B4" s="1" t="s">
         <v>71</v>
       </c>
@@ -711,7 +707,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>2</v>
       </c>
@@ -749,7 +745,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B6" t="s">
         <v>53</v>
       </c>
@@ -784,7 +780,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>8</v>
       </c>
@@ -834,7 +830,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>35</v>
       </c>
@@ -884,7 +880,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>50</v>
       </c>
@@ -931,7 +927,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>41</v>
       </c>
@@ -978,7 +974,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>47</v>
       </c>
@@ -1025,7 +1021,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>24</v>
       </c>
@@ -1072,7 +1068,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>37</v>
       </c>
@@ -1119,7 +1115,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>36</v>
       </c>
@@ -1152,7 +1148,7 @@
       </c>
       <c r="K14" s="2"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>74</v>
       </c>
@@ -1199,7 +1195,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>75</v>
       </c>
@@ -1246,7 +1242,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>46</v>
       </c>
@@ -1293,7 +1289,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>40</v>
       </c>
@@ -1340,7 +1336,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>23</v>
       </c>
@@ -1387,7 +1383,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>34</v>
       </c>
@@ -1420,7 +1416,7 @@
       </c>
       <c r="K20" s="2"/>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>43</v>
       </c>
@@ -1453,7 +1449,7 @@
       </c>
       <c r="K21" s="2"/>
     </row>
-    <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>45</v>
       </c>
@@ -1491,7 +1487,7 @@
         <v>51</v>
       </c>
       <c r="M22" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N22" s="3" t="s">
         <v>27</v>
@@ -1500,7 +1496,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="23" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>42</v>
       </c>
@@ -1538,7 +1534,7 @@
         <v>51</v>
       </c>
       <c r="M23" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N23" s="3" t="s">
         <v>27</v>
@@ -1547,7 +1543,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>39</v>
       </c>
@@ -1594,7 +1590,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="25" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>83</v>
       </c>
@@ -1641,7 +1637,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="26" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>49</v>
       </c>
@@ -1688,7 +1684,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="27" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>44</v>
       </c>
@@ -1735,7 +1731,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="28" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>48</v>
       </c>
@@ -1773,7 +1769,7 @@
         <v>51</v>
       </c>
       <c r="M28" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="N28" s="3" t="s">
         <v>27</v>
@@ -1782,7 +1778,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="29" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:15" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>38</v>
       </c>
@@ -1823,14 +1819,14 @@
         <v>0</v>
       </c>
       <c r="N29" s="3" t="s">
-        <v>27</v>
+        <v>84</v>
       </c>
       <c r="O29" s="3" t="s">
         <v>81</v>
       </c>
     </row>
   </sheetData>
-  <sortState ref="A8:O26">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A8:O26">
     <sortCondition ref="A6:A24"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>